<commit_message>
[+] Lates updates on UCID
</commit_message>
<xml_diff>
--- a/Team_3_UCID_Itteration2Update.xlsx
+++ b/Team_3_UCID_Itteration2Update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hediemoradi/Repos/SE-1-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84D8544F-CFA5-E545-9BB0-09FA6F0FE1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDFC77AB-BC2D-614F-B06F-432ADD6360CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="700" windowWidth="28360" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="700" windowWidth="16400" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="140">
   <si>
     <t>Function Name</t>
   </si>
@@ -113,17 +115,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-First name
-Last name
-Phone
-Email
-Password
-Address
-Payment information
-</t>
-  </si>
-  <si>
     <t>The System User indicates that he wants to modify the System User profile while viewing it. This function is performed after performing the View Profile function. The output is updated after a confirmation message.</t>
   </si>
   <si>
@@ -138,58 +129,16 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-None</t>
-  </si>
-  <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>View Available Vehicles</t>
   </si>
   <si>
     <t>Vending Manager</t>
   </si>
   <si>
-    <t xml:space="preserve">This function provides a list of vehicles available for next day sorted by location(ASC). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Operators Names                           
-Vehicle Name                                 
-Vehicle Type                                   
-Location ID                                    
-Ending Time
-</t>
-  </si>
-  <si>
-    <t>This function provides details of vehicle operator including his name, vehicle type, location Id, name and end time of vehicle assigned to the operator</t>
-  </si>
-  <si>
     <t>Assign Location</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Vehicle name 
-Location ID  
-Date (default to next day)
-</t>
-  </si>
-  <si>
-    <t>The System User assigns a location to the vehicle for the next day with the confirmation message.</t>
-  </si>
-  <si>
     <t>Assign Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Vehicle Name                                       
-Operator Name                                            
-Time Duration (default to entire next day)
-</t>
-  </si>
-  <si>
-    <t>The System user assigns operator to the vending vehicle for the entire next day. Assignment is successfully executed with a confirmation message</t>
   </si>
   <si>
     <t xml:space="preserve">Student/ Staff/ Faculty/non-student, </t>
@@ -210,44 +159,10 @@
     <t xml:space="preserve">Checkout </t>
   </si>
   <si>
-    <t>Payment summary
-Item name
-Quantity
-Total cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-User can review the order. If the payment methods is not added during the registration, user is prompted to add payment information. The user can place the order and successful message will be displayed. 
-</t>
-  </si>
-  <si>
-    <t>Add Payment Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Name On Card 
-Card Number 
-CVV
-Expiration date
-</t>
-  </si>
-  <si>
     <t>Vending Operator</t>
   </si>
   <si>
     <t>This function provides the schedule and location of vending operator for current day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Operator's Name                            
-Vehicle Name                                
-Vehicle Type                                   
-Location ID                                     
-Ending Time
-</t>
-  </si>
-  <si>
-    <t>No input is required because the System User selects this function after viewing a specific vehicle. Data shown as output is updated after system user confirms the save of modified data.</t>
   </si>
   <si>
     <t xml:space="preserve">Location ID, 
@@ -274,26 +189,10 @@
     <t>Accessable from all screens(not login or registration)</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Item Name                                      
-Item Type                                        
-Quantity 
-Cost (idv)
-Total cost   
-                           </t>
-  </si>
-  <si>
     <t>Checkout screen</t>
   </si>
   <si>
     <t>Payment screen</t>
-  </si>
-  <si>
-    <t>This function is performed after checkout, if payment method is not added. User can successfully add the card to the specific User profile. Then user can purchase an item. Order conformation number will be given to the user.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modify operator screen
-Manger can also navigate back to the home screen </t>
   </si>
   <si>
     <t xml:space="preserve">Modify location screen
@@ -304,29 +203,6 @@
   </si>
   <si>
     <t>View Inventory</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">View Operator screen
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF262626"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>User may also navigate back to Home screen</t>
-    </r>
-  </si>
-  <si>
-    <t>View Assign screen. 
-User may also navigate back to Home screen</t>
-  </si>
-  <si>
-    <t>View Assign screen.
-User may also navigate back to  Home screen</t>
   </si>
   <si>
     <t>Application Sign Up/ registration Screen</t>
@@ -500,11 +376,6 @@
     <t>View Operator</t>
   </si>
   <si>
-    <t xml:space="preserve">
-This function provides a list of vehicle, locations, ending time, and  operator name. This list has selectable options to show inventory for each vehicle.
-</t>
-  </si>
-  <si>
     <t>View/ Modify Vehicle Inventory</t>
   </si>
   <si>
@@ -568,11 +439,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-View Vehicle Revenue
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">View Vehicle Revenue Screen </t>
   </si>
   <si>
@@ -585,9 +451,6 @@
   </si>
   <si>
     <t xml:space="preserve">View vehicle Revenue screem. User can navigate back to home screen with using bottom navigation. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This function provides the revenue per each vehicle as well as sum of all revenues from all vehicles. </t>
   </si>
   <si>
     <t>View Location</t>
@@ -646,6 +509,153 @@
     <t>NOTE: To address all comments and feedbacks which our team received after Iteration 1, we decided to shuffle our UCID and do our best to match all the wordings,
 functions, and attributes with other documents. With these changes, we are hoping to provide clarity for you and limit any further confusion. Therefore, since most of the rows have been effected
 we decided to provide this note instead of highlighting everything and kindly ask you to review them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+User can review the order. This screen will guide the user to the payment screen by default to finish the order. If the user wishes to change the order he needs to navigate back to cart.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Cart Summary:                                      
+Item Type                                        
+Quantity 
+Cost (idv)
+Total cost   
+                           </t>
+  </si>
+  <si>
+    <t>Payment Summary:
+Item(s) name
+Quantity(s)
+Total cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Card Summary:
+Name On Card 
+Card Number 
+CVV
+Expiration date
+</t>
+  </si>
+  <si>
+    <t>Add/ Modify Card Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This function is performed after checkout. If the payment methods is not added in profile, user is prompted to add payment information. If the card information has been already added, we will propmt the user to conform the card or modify it as they want. Then user can complete his purchase. Order conformation number will be given to the user after the payment is done. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+First name
+Last name
+Phone
+Email
+Address
+Card/ Payment information
+</t>
+  </si>
+  <si>
+    <t>Assign Vehicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+View Vehicles Revenue
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Operators Names                           
+Vehicle Name                                 
+Location                                    
+Slot Begin
+Slot End
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">View Operator screen
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>User may also navigate back to Home screen from bottom navigation</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">This function provides details of vehicle and the assign operator to it. It includs operator name, vehicle type, location, begin and end time of vehicle. Manager can uodate the vehicle assigned to the operator from here. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Vehicle Name                       
+Vehicle ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+None- Date (default to next day)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Location ID  
+Location Address
+Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+None- Date (default to entire next day)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Operator ID
+Operator Name
+</t>
+  </si>
+  <si>
+    <t>Assign Time Slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start time (Slot Begin)
+End time (Slot End)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assign screen.
+User may also navigate back to  Home screen from bottom navigation</t>
+  </si>
+  <si>
+    <t>Assign screen. 
+User may also navigate back to Home screen  from bottom navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assign screen. 
+User may also navigate back to Home screen  from bottom navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This function provides a list of vehicles available for next day sorted by ID (ASC). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This function provides a list of Locations available for next day sorted by ID (ASC). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This function provides a list of operators available for next day sorted by ID (ASC). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This function provides a list of availible time slots for next day sorted by time (ASC). </t>
+  </si>
+  <si>
+    <t>This function provides the revenue per each vehicle as well as sum of all revenues from all vehicles. Sorted by vehicle ID (ASC) in database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+This function provides a list of vehicle, locations, ending time, and  operator name. This list has selectable options to show inventory for each vehicle. Sorted by vehicle ID (ASC) from data base. 
+</t>
   </si>
 </sst>
 </file>
@@ -1485,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="50" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -1506,7 +1516,7 @@
   <sheetData>
     <row r="1" spans="1:1025" s="60" customFormat="1" ht="102" customHeight="1">
       <c r="A1" s="59" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1025" s="51" customFormat="1" ht="48">
@@ -1521,7 +1531,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="F2" s="57" t="s">
         <v>3</v>
@@ -2561,19 +2571,19 @@
         <v>7</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1025" ht="95">
@@ -2587,7 +2597,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>11</v>
@@ -2596,10 +2606,10 @@
         <v>8</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1025" ht="95">
@@ -2607,25 +2617,25 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:1025" ht="76">
@@ -2648,10 +2658,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1025" ht="190">
@@ -2665,7 +2675,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>8</v>
@@ -2674,13 +2684,13 @@
         <v>18</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="H7" s="37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:1025" ht="171">
+    <row r="8" spans="1:1025" ht="152">
       <c r="A8" s="13">
         <v>5</v>
       </c>
@@ -2691,19 +2701,19 @@
         <v>13</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1025" s="6" customFormat="1" ht="133">
@@ -2711,25 +2721,25 @@
         <v>6</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C9" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>25</v>
-      </c>
       <c r="G9" s="32" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -3754,25 +3764,25 @@
         <v>7</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="H10" s="38" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -4797,25 +4807,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -5840,25 +5850,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -6878,30 +6888,30 @@
       <c r="AMJ12" s="5"/>
       <c r="AMK12" s="5"/>
     </row>
-    <row r="13" spans="1:1025" s="6" customFormat="1" ht="114">
+    <row r="13" spans="1:1025" s="6" customFormat="1" ht="95">
       <c r="A13" s="13">
         <v>10</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H13" s="38" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -7921,30 +7931,30 @@
       <c r="AMJ13" s="5"/>
       <c r="AMK13" s="5"/>
     </row>
-    <row r="14" spans="1:1025" s="6" customFormat="1" ht="114">
+    <row r="14" spans="1:1025" s="6" customFormat="1" ht="133">
       <c r="A14" s="13">
         <v>11</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -8969,25 +8979,25 @@
         <v>12</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -10012,25 +10022,25 @@
         <v>13</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -11050,30 +11060,30 @@
       <c r="AMJ16" s="8"/>
       <c r="AMK16" s="8"/>
     </row>
-    <row r="17" spans="1:1025" s="9" customFormat="1" ht="133">
+    <row r="17" spans="1:1025" s="9" customFormat="1" ht="114">
       <c r="A17" s="13">
         <v>14</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -12093,30 +12103,30 @@
       <c r="AMJ17" s="8"/>
       <c r="AMK17" s="8"/>
     </row>
-    <row r="18" spans="1:1025" s="9" customFormat="1" ht="190">
+    <row r="18" spans="1:1025" s="9" customFormat="1" ht="57">
       <c r="A18" s="13">
         <v>15</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
       <c r="H18" s="39" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -13136,30 +13146,30 @@
       <c r="AMJ18" s="8"/>
       <c r="AMK18" s="8"/>
     </row>
-    <row r="19" spans="1:1025" s="9" customFormat="1" ht="133">
+    <row r="19" spans="1:1025" s="9" customFormat="1" ht="76">
       <c r="A19" s="13">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="H19" s="39" t="s">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -14179,30 +14189,30 @@
       <c r="AMJ19" s="8"/>
       <c r="AMK19" s="8"/>
     </row>
-    <row r="20" spans="1:1025" s="9" customFormat="1" ht="95">
+    <row r="20" spans="1:1025" s="9" customFormat="1" ht="76">
       <c r="A20" s="13">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
-      <c r="D20" s="42" t="s">
-        <v>55</v>
+      <c r="D20" s="43" t="s">
+        <v>39</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
-      <c r="G20" s="32" t="s">
-        <v>67</v>
+      <c r="G20" s="33" t="s">
+        <v>132</v>
       </c>
       <c r="H20" s="39" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -15222,30 +15232,30 @@
       <c r="AMJ20" s="8"/>
       <c r="AMK20" s="8"/>
     </row>
-    <row r="21" spans="1:1025" s="9" customFormat="1" ht="114">
+    <row r="21" spans="1:1025" s="9" customFormat="1" ht="57">
       <c r="A21" s="13">
         <v>18</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -16267,28 +16277,28 @@
     </row>
     <row r="22" spans="1:1025" s="9" customFormat="1" ht="133">
       <c r="A22" s="13">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="H22" s="39" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -17313,25 +17323,25 @@
         <v>20</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H23" s="39" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -18356,25 +18366,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="H24" s="39" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -19399,25 +19409,25 @@
         <v>22</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
@@ -20437,30 +20447,30 @@
       <c r="AMJ25" s="11"/>
       <c r="AMK25" s="11"/>
     </row>
-    <row r="26" spans="1:1025" s="12" customFormat="1" ht="133">
+    <row r="26" spans="1:1025" s="12" customFormat="1" ht="114">
       <c r="A26" s="13">
         <v>23</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>

</xml_diff>

<commit_message>
[+] Add XML for checkout and place order- Updated UCID
</commit_message>
<xml_diff>
--- a/Team_3_UCID_Itteration2Update.xlsx
+++ b/Team_3_UCID_Itteration2Update.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hediemoradi/Repos/SE-1-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7418BBB2-FFF3-D44D-8D4D-FCDA34990FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDB9175-BE6A-E848-8ED8-B8DC795F230E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="1000" windowWidth="13440" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="480" windowWidth="23460" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,15 +522,6 @@
                            </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Card Summary:
-Name On Card 
-Card Number 
-CVV
-Expiration date
-</t>
-  </si>
-  <si>
     <t>Add/ Modify Card Information</t>
   </si>
   <si>
@@ -677,6 +668,15 @@
   </si>
   <si>
     <t>This fuction provides the user to modify the assigned vehicle to the operator. The manager can see the list of availible vehicles from the drop down menue (sorted by vehcile id (ASC)). After the update is done the system will display a success toast message to the user and goes to view operator screen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Card Summary:
+Card Number 
+CVV
+Expiration date
+Cart type
+</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" zoomScale="84" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="31" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -1539,7 +1539,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:1025" s="51" customFormat="1" ht="48">
+    <row r="2" spans="1:1025" s="51" customFormat="1" ht="24">
       <c r="A2" s="52"/>
       <c r="B2" s="53" t="s">
         <v>0</v>
@@ -2637,7 +2637,7 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>13</v>
@@ -2727,7 +2727,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>74</v>
@@ -6925,7 +6925,7 @@
         <v>25</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G13" s="32" t="s">
         <v>67</v>
@@ -7956,7 +7956,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="45" t="s">
         <v>29</v>
@@ -7965,7 +7965,7 @@
         <v>43</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>25</v>
@@ -7974,7 +7974,7 @@
         <v>66</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -9017,7 +9017,7 @@
         <v>70</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -11085,7 +11085,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="46" t="s">
         <v>26</v>
@@ -11103,7 +11103,7 @@
         <v>95</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -12128,7 +12128,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="46" t="s">
         <v>26</v>
@@ -12140,13 +12140,13 @@
         <v>72</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H18" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -13168,7 +13168,7 @@
     </row>
     <row r="19" spans="1:1025" s="9" customFormat="1" ht="76">
       <c r="A19" s="13">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>27</v>
@@ -13180,16 +13180,16 @@
         <v>39</v>
       </c>
       <c r="E19" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="F19" s="29" t="s">
-        <v>124</v>
-      </c>
       <c r="G19" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H19" s="39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -14211,7 +14211,7 @@
     </row>
     <row r="20" spans="1:1025" s="9" customFormat="1" ht="76">
       <c r="A20" s="13">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>28</v>
@@ -14223,16 +14223,16 @@
         <v>39</v>
       </c>
       <c r="E20" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F20" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="29" t="s">
-        <v>126</v>
-      </c>
       <c r="G20" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H20" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -15257,7 +15257,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="46" t="s">
         <v>26</v>
@@ -15266,16 +15266,16 @@
         <v>39</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -16297,7 +16297,7 @@
     </row>
     <row r="22" spans="1:1025" s="9" customFormat="1" ht="133">
       <c r="A22" s="13">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>80</v>
@@ -16312,13 +16312,13 @@
         <v>25</v>
       </c>
       <c r="F22" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="H22" s="39" t="s">
         <v>120</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>121</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -17339,27 +17339,29 @@
       <c r="AMK22" s="8"/>
     </row>
     <row r="23" spans="1:1025" s="9" customFormat="1" ht="95">
-      <c r="A23" s="13"/>
+      <c r="A23" s="13">
+        <v>20</v>
+      </c>
       <c r="B23" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" s="46" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E23" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="H23" s="39" t="s">
         <v>143</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>144</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -18381,7 +18383,7 @@
     </row>
     <row r="24" spans="1:1025" s="9" customFormat="1" ht="76">
       <c r="A24" s="13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>97</v>
@@ -19424,7 +19426,7 @@
     </row>
     <row r="25" spans="1:1025" s="9" customFormat="1" ht="76">
       <c r="A25" s="13">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>96</v>
@@ -20467,7 +20469,7 @@
     </row>
     <row r="26" spans="1:1025" s="12" customFormat="1" ht="152">
       <c r="A26" s="13">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>79</v>
@@ -21510,7 +21512,7 @@
     </row>
     <row r="27" spans="1:1025" s="12" customFormat="1" ht="114">
       <c r="A27" s="13">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>81</v>

</xml_diff>